<commit_message>
corrige las tablas en excel
</commit_message>
<xml_diff>
--- a/data/cuadros/Comercio, Hoteles y Restaurantes/bh [1].xlsx
+++ b/data/cuadros/Comercio, Hoteles y Restaurantes/bh [1].xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t/>
   </si>
@@ -85,7 +85,7 @@
   <numFmts count="1">
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="451">
+  <fonts count="676">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1892,8 +1892,909 @@
       <name val="Times New Roman"/>
       <b/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <b/>
+    </font>
   </fonts>
-  <fills count="128">
+  <fills count="191">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2530,8 +3431,323 @@
         <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="351">
+  <borders count="526">
     <border>
       <left/>
       <right/>
@@ -5049,11 +6265,1266 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="351">
+  <cellXfs count="526">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
@@ -6452,6 +8923,706 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="450" fillId="0" borderId="350" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="451" fillId="0" borderId="351" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="452" fillId="0" borderId="352" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="453" fillId="0" borderId="353" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="454" fillId="0" borderId="354" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="455" fillId="0" borderId="355" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="456" fillId="0" borderId="356" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="457" fillId="0" borderId="357" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="458" fillId="0" borderId="358" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="459" fillId="0" borderId="359" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="460" fillId="0" borderId="360" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="461" fillId="0" borderId="361" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="462" fillId="0" borderId="362" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="463" fillId="0" borderId="363" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="464" fillId="0" borderId="364" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="465" fillId="0" borderId="365" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="466" fillId="0" borderId="366" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="467" fillId="0" borderId="367" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="468" fillId="0" borderId="368" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="469" fillId="0" borderId="369" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="470" fillId="0" borderId="370" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="471" fillId="0" borderId="371" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="472" fillId="0" borderId="372" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="473" fillId="0" borderId="373" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="474" fillId="0" borderId="374" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="475" fillId="0" borderId="375" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="476" fillId="0" borderId="376" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="477" fillId="0" borderId="377" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="478" fillId="0" borderId="378" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="479" fillId="0" borderId="379" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="480" fillId="0" borderId="380" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="481" fillId="0" borderId="381" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="482" fillId="0" borderId="382" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="483" fillId="0" borderId="383" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="484" fillId="0" borderId="384" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="485" fillId="0" borderId="385" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="486" fillId="0" borderId="386" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="487" fillId="0" borderId="387" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="488" fillId="0" borderId="388" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="489" fillId="0" borderId="389" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="490" fillId="0" borderId="390" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="491" fillId="0" borderId="391" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="492" fillId="0" borderId="392" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="493" fillId="0" borderId="393" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="494" fillId="0" borderId="394" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="495" fillId="0" borderId="395" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="496" fillId="0" borderId="396" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="497" fillId="0" borderId="397" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="498" fillId="0" borderId="398" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="499" fillId="0" borderId="399" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="500" fillId="0" borderId="400" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="501" fillId="0" borderId="401" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="502" fillId="0" borderId="402" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="503" fillId="0" borderId="403" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="504" fillId="0" borderId="404" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="505" fillId="0" borderId="405" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="506" fillId="0" borderId="406" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="507" fillId="0" borderId="407" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="508" fillId="0" borderId="408" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="509" fillId="0" borderId="409" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="510" fillId="0" borderId="410" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="511" fillId="0" borderId="411" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="512" fillId="0" borderId="412" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="514" fillId="0" borderId="413" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="516" fillId="0" borderId="414" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="518" fillId="0" borderId="415" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="520" fillId="0" borderId="416" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="522" fillId="0" borderId="417" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="524" fillId="0" borderId="418" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="526" fillId="0" borderId="419" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="528" fillId="0" borderId="420" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="530" fillId="0" borderId="421" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="532" fillId="0" borderId="422" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="534" fillId="0" borderId="423" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="536" fillId="0" borderId="424" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="538" fillId="0" borderId="425" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="540" fillId="0" borderId="426" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="542" fillId="0" borderId="427" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="544" fillId="0" borderId="428" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="546" fillId="0" borderId="429" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="548" fillId="0" borderId="430" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="550" fillId="0" borderId="431" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="552" fillId="0" borderId="432" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="554" fillId="0" borderId="433" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="556" fillId="0" borderId="434" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="558" fillId="0" borderId="435" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="560" fillId="0" borderId="436" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="562" fillId="0" borderId="437" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="564" fillId="0" borderId="438" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="566" fillId="0" borderId="439" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="568" fillId="0" borderId="440" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="570" fillId="0" borderId="441" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="572" fillId="0" borderId="442" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="574" fillId="0" borderId="443" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="576" fillId="0" borderId="444" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="578" fillId="0" borderId="445" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="580" fillId="0" borderId="446" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="582" fillId="0" borderId="447" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="584" fillId="0" borderId="448" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="586" fillId="0" borderId="449" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="588" fillId="0" borderId="450" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="590" fillId="0" borderId="451" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="592" fillId="0" borderId="452" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="594" fillId="0" borderId="453" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="596" fillId="0" borderId="454" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="598" fillId="0" borderId="455" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="600" fillId="0" borderId="456" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="602" fillId="0" borderId="457" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="604" fillId="0" borderId="458" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="606" fillId="0" borderId="459" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="608" fillId="0" borderId="460" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="609" fillId="128" borderId="461" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="610" fillId="129" borderId="462" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="611" fillId="130" borderId="463" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="612" fillId="131" borderId="464" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="613" fillId="132" borderId="465" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="614" fillId="133" borderId="466" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="615" fillId="134" borderId="467" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="616" fillId="135" borderId="468" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="617" fillId="136" borderId="469" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="618" fillId="137" borderId="470" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="619" fillId="138" borderId="471" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="620" fillId="139" borderId="472" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="621" fillId="140" borderId="473" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="622" fillId="141" borderId="474" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="623" fillId="142" borderId="475" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="624" fillId="143" borderId="476" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="625" fillId="144" borderId="477" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="626" fillId="145" borderId="478" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="627" fillId="146" borderId="479" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="628" fillId="147" borderId="480" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="629" fillId="148" borderId="481" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="630" fillId="149" borderId="482" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="631" fillId="150" borderId="483" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="632" fillId="151" borderId="484" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="633" fillId="152" borderId="485" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="634" fillId="153" borderId="486" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="635" fillId="154" borderId="487" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="636" fillId="155" borderId="488" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="637" fillId="156" borderId="489" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="638" fillId="157" borderId="490" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="639" fillId="158" borderId="491" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="640" fillId="159" borderId="492" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="641" fillId="160" borderId="493" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="642" fillId="161" borderId="494" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="643" fillId="162" borderId="495" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="644" fillId="163" borderId="496" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="645" fillId="164" borderId="497" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="646" fillId="165" borderId="498" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="647" fillId="166" borderId="499" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="648" fillId="167" borderId="500" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="649" fillId="168" borderId="501" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="650" fillId="169" borderId="502" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="651" fillId="170" borderId="503" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="652" fillId="171" borderId="504" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="653" fillId="172" borderId="505" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="654" fillId="173" borderId="506" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="655" fillId="174" borderId="507" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="656" fillId="175" borderId="508" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="657" fillId="176" borderId="509" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="658" fillId="177" borderId="510" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="659" fillId="178" borderId="511" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="660" fillId="179" borderId="512" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="661" fillId="180" borderId="513" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="662" fillId="181" borderId="514" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="663" fillId="182" borderId="515" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="664" fillId="183" borderId="516" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="665" fillId="184" borderId="517" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="666" fillId="185" borderId="518" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="667" fillId="186" borderId="519" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="668" fillId="187" borderId="520" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="669" fillId="188" borderId="521" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="670" fillId="189" borderId="522" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="671" fillId="190" borderId="523" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="673" fillId="0" borderId="524" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="675" fillId="0" borderId="525" xfId="0" applyNumberFormat="true" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -6468,184 +9639,184 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="350" t="s">
+      <c r="A1" s="525" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="346" t="s">
+      <c r="A2" s="521" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="347" t="s">
+      <c r="B2" s="522" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="348" t="s">
+      <c r="C2" s="523" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="464" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="290">
+      <c r="B3" s="465">
         <v>27.600000000000001</v>
       </c>
-      <c r="C3" s="291">
-        <v>13.300000000000001</v>
+      <c r="C3" s="466">
+        <v>14</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="292" t="s">
+      <c r="A4" s="467" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="293">
+      <c r="B4" s="468">
         <v>23.300000000000001</v>
       </c>
-      <c r="C4" s="294">
-        <v>14.100000000000001</v>
+      <c r="C4" s="469">
+        <v>15.100000000000001</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="295" t="s">
+      <c r="A5" s="470" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="296">
+      <c r="B5" s="471">
         <v>16.699999999999999</v>
       </c>
-      <c r="C5" s="297">
-        <v>4.6000000000000005</v>
+      <c r="C5" s="472">
+        <v>4.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="298" t="s">
+      <c r="A6" s="473" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="299">
+      <c r="B6" s="474">
         <v>21.600000000000001</v>
       </c>
-      <c r="C6" s="300">
+      <c r="C6" s="475">
         <v>5.6000000000000005</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="301" t="s">
+      <c r="A7" s="476" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="302">
+      <c r="B7" s="477">
         <v>24.400000000000002</v>
       </c>
-      <c r="C7" s="303">
+      <c r="C7" s="478">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="479" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="480">
+        <v>24.900000000000002</v>
+      </c>
+      <c r="C8" s="481">
+        <v>8.2000000000000011</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="482" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="483">
+        <v>25.5</v>
+      </c>
+      <c r="C9" s="484">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="485" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="486">
+        <v>20.600000000000001</v>
+      </c>
+      <c r="C10" s="487">
+        <v>6.6000000000000005</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="488" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="489">
+        <v>21.700000000000003</v>
+      </c>
+      <c r="C11" s="490">
         <v>8.9000000000000004</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="304" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="305">
-        <v>24.900000000000002</v>
-      </c>
-      <c r="C8" s="306">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="307" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="308">
-        <v>25.5</v>
-      </c>
-      <c r="C9" s="309">
-        <v>15.100000000000001</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="310" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="311">
-        <v>20.600000000000001</v>
-      </c>
-      <c r="C10" s="312">
-        <v>6.2000000000000002</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="313" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="314">
-        <v>21.700000000000003</v>
-      </c>
-      <c r="C11" s="315">
-        <v>9.3000000000000007</v>
-      </c>
-    </row>
     <row r="12">
-      <c r="A12" s="316" t="s">
+      <c r="A12" s="491" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="317">
+      <c r="B12" s="492">
         <v>23.800000000000001</v>
       </c>
-      <c r="C12" s="318">
-        <v>8.4000000000000004</v>
+      <c r="C12" s="493">
+        <v>8.5</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="319" t="s">
+      <c r="A13" s="494" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="320">
+      <c r="B13" s="495">
         <v>21.800000000000001</v>
       </c>
-      <c r="C13" s="321">
-        <v>10.9</v>
+      <c r="C13" s="496">
+        <v>11.9</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="322" t="s">
+      <c r="A14" s="497" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="323">
+      <c r="B14" s="498">
         <v>17.100000000000001</v>
       </c>
-      <c r="C14" s="324">
-        <v>10.600000000000001</v>
+      <c r="C14" s="499">
+        <v>11.9</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="325" t="s">
+      <c r="A15" s="500" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="326">
+      <c r="B15" s="501">
         <v>21.5</v>
       </c>
-      <c r="C15" s="327">
-        <v>9</v>
+      <c r="C15" s="502">
+        <v>10.700000000000001</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="340" t="s">
+      <c r="A16" s="515" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="341">
+      <c r="B16" s="516">
         <v>18.300000000000001</v>
       </c>
-      <c r="C16" s="342">
-        <v>5.7000000000000002</v>
+      <c r="C16" s="517">
+        <v>6.5</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="343" t="s">
+      <c r="A17" s="518" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="344">
+      <c r="B17" s="519">
         <v>20.300000000000001</v>
       </c>
-      <c r="C17" s="345">
-        <v>11.9</v>
+      <c r="C17" s="520">
+        <v>12.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>